<commit_message>
balancing for AFVs, heavy AT, additional loc for AFV modules
</commit_message>
<xml_diff>
--- a/Modding resources/Land combat/Eq_stats_md.xlsx
+++ b/Modding resources/Land combat/Eq_stats_md.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Old stats" sheetId="1" r:id="rId1"/>
     <sheet name="New stats" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="193">
   <si>
     <t>Identification</t>
   </si>
@@ -602,6 +603,18 @@
   </si>
   <si>
     <t>L inf div 2005</t>
+  </si>
+  <si>
+    <t>apc 1965</t>
+  </si>
+  <si>
+    <t>apc 1975</t>
+  </si>
+  <si>
+    <t>apc 1995</t>
+  </si>
+  <si>
+    <t>ifv 1965</t>
   </si>
 </sst>
 </file>
@@ -742,7 +755,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -890,11 +903,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -953,6 +1074,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8832,8 +8969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15965,4 +16102,1725 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="46">
+        <v>1</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="46">
+        <v>2</v>
+      </c>
+      <c r="G3" s="46">
+        <v>3</v>
+      </c>
+      <c r="H3" s="46">
+        <v>0</v>
+      </c>
+      <c r="I3" s="46">
+        <v>4</v>
+      </c>
+      <c r="J3" s="46">
+        <v>3</v>
+      </c>
+      <c r="K3" s="46">
+        <v>5</v>
+      </c>
+      <c r="L3" s="46">
+        <v>5</v>
+      </c>
+      <c r="M3" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="N3" s="46">
+        <v>8.5</v>
+      </c>
+      <c r="O3" s="46">
+        <v>0.9</v>
+      </c>
+      <c r="P3" s="48">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="47">
+        <v>2</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="47">
+        <v>2.5</v>
+      </c>
+      <c r="G4" s="47">
+        <v>3.75</v>
+      </c>
+      <c r="H4" s="47">
+        <v>0</v>
+      </c>
+      <c r="I4" s="47">
+        <v>7</v>
+      </c>
+      <c r="J4" s="47">
+        <v>5</v>
+      </c>
+      <c r="K4" s="47">
+        <v>5.5</v>
+      </c>
+      <c r="L4" s="47">
+        <v>9</v>
+      </c>
+      <c r="M4" s="47">
+        <v>0.4</v>
+      </c>
+      <c r="N4" s="47">
+        <v>9</v>
+      </c>
+      <c r="O4" s="47">
+        <v>0.9</v>
+      </c>
+      <c r="P4" s="49">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="46">
+        <v>3</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="46">
+        <v>3</v>
+      </c>
+      <c r="G5" s="46">
+        <v>4.5</v>
+      </c>
+      <c r="H5" s="46">
+        <v>0</v>
+      </c>
+      <c r="I5" s="46">
+        <v>10</v>
+      </c>
+      <c r="J5" s="46">
+        <v>7</v>
+      </c>
+      <c r="K5" s="46">
+        <v>6</v>
+      </c>
+      <c r="L5" s="46">
+        <v>13</v>
+      </c>
+      <c r="M5" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="N5" s="46">
+        <v>9.5</v>
+      </c>
+      <c r="O5" s="46">
+        <v>0.9</v>
+      </c>
+      <c r="P5" s="48">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="52">
+        <v>4</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="52">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="52">
+        <v>5.25</v>
+      </c>
+      <c r="H6" s="52">
+        <v>0</v>
+      </c>
+      <c r="I6" s="52">
+        <v>13</v>
+      </c>
+      <c r="J6" s="52">
+        <v>9</v>
+      </c>
+      <c r="K6" s="52">
+        <v>6.5</v>
+      </c>
+      <c r="L6" s="52">
+        <v>17</v>
+      </c>
+      <c r="M6" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="N6" s="52">
+        <v>10</v>
+      </c>
+      <c r="O6" s="52">
+        <v>0.9</v>
+      </c>
+      <c r="P6" s="58">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="55">
+        <v>5</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="55">
+        <v>4</v>
+      </c>
+      <c r="G7" s="55">
+        <v>6</v>
+      </c>
+      <c r="H7" s="55">
+        <v>0</v>
+      </c>
+      <c r="I7" s="55">
+        <v>16</v>
+      </c>
+      <c r="J7" s="55">
+        <v>13</v>
+      </c>
+      <c r="K7" s="55">
+        <v>7</v>
+      </c>
+      <c r="L7" s="55">
+        <v>21</v>
+      </c>
+      <c r="M7" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="N7" s="55">
+        <v>10.5</v>
+      </c>
+      <c r="O7" s="55">
+        <v>0.9</v>
+      </c>
+      <c r="P7" s="57">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="52">
+        <v>6</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="52">
+        <v>4.5</v>
+      </c>
+      <c r="G8" s="52">
+        <v>6.75</v>
+      </c>
+      <c r="H8" s="52">
+        <v>0</v>
+      </c>
+      <c r="I8" s="52">
+        <v>19</v>
+      </c>
+      <c r="J8" s="52">
+        <v>15</v>
+      </c>
+      <c r="K8" s="52">
+        <v>7.5</v>
+      </c>
+      <c r="L8" s="52">
+        <v>25</v>
+      </c>
+      <c r="M8" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="52">
+        <v>11</v>
+      </c>
+      <c r="O8" s="52">
+        <v>0.9</v>
+      </c>
+      <c r="P8" s="58">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="55">
+        <v>7</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="55">
+        <v>5</v>
+      </c>
+      <c r="G9" s="55">
+        <v>7.5</v>
+      </c>
+      <c r="H9" s="55">
+        <v>0</v>
+      </c>
+      <c r="I9" s="55">
+        <v>22</v>
+      </c>
+      <c r="J9" s="55">
+        <v>17</v>
+      </c>
+      <c r="K9" s="55">
+        <v>8</v>
+      </c>
+      <c r="L9" s="55">
+        <v>29</v>
+      </c>
+      <c r="M9" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="N9" s="55">
+        <v>11.5</v>
+      </c>
+      <c r="O9" s="55">
+        <v>0.9</v>
+      </c>
+      <c r="P9" s="57">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="47">
+        <v>8</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="47">
+        <v>5.5</v>
+      </c>
+      <c r="G10" s="47">
+        <v>8.25</v>
+      </c>
+      <c r="H10" s="47">
+        <v>0</v>
+      </c>
+      <c r="I10" s="47">
+        <v>25</v>
+      </c>
+      <c r="J10" s="52">
+        <v>19</v>
+      </c>
+      <c r="K10" s="52">
+        <v>8.5</v>
+      </c>
+      <c r="L10" s="52">
+        <v>33</v>
+      </c>
+      <c r="M10" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="N10" s="52">
+        <v>12</v>
+      </c>
+      <c r="O10" s="52">
+        <v>0.9</v>
+      </c>
+      <c r="P10" s="58">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="46">
+        <v>1</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="46">
+        <v>4</v>
+      </c>
+      <c r="G11" s="46">
+        <v>7</v>
+      </c>
+      <c r="H11" s="46">
+        <v>0</v>
+      </c>
+      <c r="I11" s="46">
+        <v>15</v>
+      </c>
+      <c r="J11" s="55">
+        <v>6</v>
+      </c>
+      <c r="K11" s="55">
+        <v>6</v>
+      </c>
+      <c r="L11" s="55">
+        <v>5</v>
+      </c>
+      <c r="M11" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="55">
+        <v>8.5</v>
+      </c>
+      <c r="O11" s="55">
+        <v>0.9</v>
+      </c>
+      <c r="P11" s="57">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="47">
+        <v>2</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="47">
+        <v>5</v>
+      </c>
+      <c r="G12" s="47">
+        <v>9</v>
+      </c>
+      <c r="H12" s="47">
+        <v>0</v>
+      </c>
+      <c r="I12" s="47">
+        <v>19</v>
+      </c>
+      <c r="J12" s="47">
+        <v>9</v>
+      </c>
+      <c r="K12" s="47">
+        <v>6.75</v>
+      </c>
+      <c r="L12" s="52">
+        <v>9</v>
+      </c>
+      <c r="M12" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="52">
+        <v>9</v>
+      </c>
+      <c r="O12" s="52">
+        <v>0.9</v>
+      </c>
+      <c r="P12" s="58">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="46">
+        <v>3</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="46">
+        <v>6</v>
+      </c>
+      <c r="G13" s="46">
+        <v>11</v>
+      </c>
+      <c r="H13" s="46">
+        <v>0</v>
+      </c>
+      <c r="I13" s="46">
+        <v>23</v>
+      </c>
+      <c r="J13" s="46">
+        <v>12</v>
+      </c>
+      <c r="K13" s="46">
+        <v>7.5</v>
+      </c>
+      <c r="L13" s="55">
+        <v>13</v>
+      </c>
+      <c r="M13" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="N13" s="55">
+        <v>9.5</v>
+      </c>
+      <c r="O13" s="55">
+        <v>0.9</v>
+      </c>
+      <c r="P13" s="57">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="52">
+        <v>4</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="47">
+        <v>7</v>
+      </c>
+      <c r="G14" s="52">
+        <v>13</v>
+      </c>
+      <c r="H14" s="47">
+        <v>0</v>
+      </c>
+      <c r="I14" s="52">
+        <v>27</v>
+      </c>
+      <c r="J14" s="47">
+        <v>15</v>
+      </c>
+      <c r="K14" s="47">
+        <v>8.25</v>
+      </c>
+      <c r="L14" s="52">
+        <v>17</v>
+      </c>
+      <c r="M14" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="N14" s="52">
+        <v>10</v>
+      </c>
+      <c r="O14" s="52">
+        <v>0.9</v>
+      </c>
+      <c r="P14" s="58">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="55">
+        <v>5</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="55">
+        <v>8</v>
+      </c>
+      <c r="G15" s="55">
+        <v>15</v>
+      </c>
+      <c r="H15" s="55">
+        <v>0</v>
+      </c>
+      <c r="I15" s="55">
+        <v>31</v>
+      </c>
+      <c r="J15" s="55">
+        <v>18</v>
+      </c>
+      <c r="K15" s="55">
+        <v>9</v>
+      </c>
+      <c r="L15" s="55">
+        <v>21</v>
+      </c>
+      <c r="M15" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="N15" s="55">
+        <v>10.5</v>
+      </c>
+      <c r="O15" s="55">
+        <v>0.9</v>
+      </c>
+      <c r="P15" s="57">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="52">
+        <v>6</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="52">
+        <v>9</v>
+      </c>
+      <c r="G16" s="52">
+        <v>17</v>
+      </c>
+      <c r="H16" s="52">
+        <v>0</v>
+      </c>
+      <c r="I16" s="52">
+        <v>35</v>
+      </c>
+      <c r="J16" s="52">
+        <v>21</v>
+      </c>
+      <c r="K16" s="52">
+        <v>9.75</v>
+      </c>
+      <c r="L16" s="52">
+        <v>25</v>
+      </c>
+      <c r="M16" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="N16" s="52">
+        <v>11</v>
+      </c>
+      <c r="O16" s="52">
+        <v>0.9</v>
+      </c>
+      <c r="P16" s="58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="46">
+        <v>7</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="46">
+        <v>10</v>
+      </c>
+      <c r="G17" s="55">
+        <v>19</v>
+      </c>
+      <c r="H17" s="46">
+        <v>0</v>
+      </c>
+      <c r="I17" s="55">
+        <v>39</v>
+      </c>
+      <c r="J17" s="46">
+        <v>24</v>
+      </c>
+      <c r="K17" s="46">
+        <v>10.5</v>
+      </c>
+      <c r="L17" s="55">
+        <v>29</v>
+      </c>
+      <c r="M17" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="N17" s="55">
+        <v>11.5</v>
+      </c>
+      <c r="O17" s="55">
+        <v>0.9</v>
+      </c>
+      <c r="P17" s="48">
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="52">
+        <v>8</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="52">
+        <v>11</v>
+      </c>
+      <c r="G18" s="52">
+        <v>21</v>
+      </c>
+      <c r="H18" s="52">
+        <v>0</v>
+      </c>
+      <c r="I18" s="52">
+        <v>42</v>
+      </c>
+      <c r="J18" s="52">
+        <v>27</v>
+      </c>
+      <c r="K18" s="52">
+        <v>11.25</v>
+      </c>
+      <c r="L18" s="52">
+        <v>33</v>
+      </c>
+      <c r="M18" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="N18" s="52">
+        <v>12</v>
+      </c>
+      <c r="O18" s="52">
+        <v>0.9</v>
+      </c>
+      <c r="P18" s="49">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>9</v>
+      </c>
+      <c r="N21">
+        <v>11</v>
+      </c>
+      <c r="P21">
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>190</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>11</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="N22">
+        <v>15</v>
+      </c>
+      <c r="P22">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <v>17</v>
+      </c>
+      <c r="N23">
+        <v>16.8</v>
+      </c>
+      <c r="P23">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26">
+        <v>12</v>
+      </c>
+      <c r="G26">
+        <v>9.5</v>
+      </c>
+      <c r="I26">
+        <v>12</v>
+      </c>
+      <c r="J26">
+        <v>11</v>
+      </c>
+      <c r="K26">
+        <v>17</v>
+      </c>
+      <c r="L26">
+        <v>9</v>
+      </c>
+      <c r="N26">
+        <v>13</v>
+      </c>
+      <c r="P26">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>12.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="dataBar" priority="29">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{24353EF2-2E4E-47D9-BB13-AF33DD814C27}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F10">
+    <cfRule type="dataBar" priority="28">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C984249B-7577-42FB-8C6B-39488E7067F2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G10">
+    <cfRule type="dataBar" priority="27">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2B40E5D8-A379-457C-81F5-3175CFE24036}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H10">
+    <cfRule type="dataBar" priority="26">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6CF82327-A02F-40B6-A0ED-D563C11BD860}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I10">
+    <cfRule type="dataBar" priority="25">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D307157D-C90A-44CF-B7BF-29610E62CF3D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J10">
+    <cfRule type="dataBar" priority="24">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AF520A82-3C00-40DA-8F14-1EF756F6BE27}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K10">
+    <cfRule type="dataBar" priority="23">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BDB0AC50-6326-4FE2-8EBB-A9645CA60DCF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L10">
+    <cfRule type="dataBar" priority="22">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{56390780-E899-46CA-BB7D-2D0CB4C306C7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M10">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{82AE36BD-71E3-4179-BBA8-F08783EAFE7E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N10">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D7B4FE4C-543C-42AB-8CED-20BCB22D01C1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O10">
+    <cfRule type="dataBar" priority="19">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8E53F878-39C8-4364-9202-725B88D49B9D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P10">
+    <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{59F14498-126E-4615-96AE-185AD5F0025D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P10">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{89478E4F-2919-4C59-A4F1-F83163F8AE49}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P10">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{86EF0297-B943-4257-AE8A-BC47340A1EEC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P10">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3FF5350B-37FD-4627-AA01-A649A47D3864}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F18">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A6E7E027-47DE-4B49-8931-80A2B606B734}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G18">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CF525180-9BAE-4A80-9AF8-0A4183AA4731}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:H18">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{88FC12ED-70BD-4AA3-ABC4-D1638E18C917}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I18">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{03C53742-1396-49B5-A75C-B8F2EE6DF507}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J18">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E53703C8-6EC4-45AF-A7C5-27EB0E1EDB3C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11:K18">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EC2ACDAC-3433-4298-BB56-4CD282E2FDE1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11:L18">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5F1B9428-DA36-4346-92C6-B774C6ADB83F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M18">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8622EB6C-D203-44D6-97DC-BB9E83F74AA9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11:N18">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{54098384-335C-438C-878E-434B302F1C30}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11:O18">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D7C9DAAE-A316-4507-9935-7E8B7A6D9000}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P11:P18">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7305E562-99D7-4701-A3CB-673F89DF4A6E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P11:P18">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8721FE99-682B-4CD0-949A-B19E552FB3F2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P11:P18">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7AF7AED4-59B8-40E1-824C-CE7010BF7176}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P11:P18">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{38EA70F9-0A79-4BED-8545-D678A2A1186D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{24353EF2-2E4E-47D9-BB13-AF33DD814C27}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C984249B-7577-42FB-8C6B-39488E7067F2}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F3:F10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2B40E5D8-A379-457C-81F5-3175CFE24036}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G3:G10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6CF82327-A02F-40B6-A0ED-D563C11BD860}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H3:H10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D307157D-C90A-44CF-B7BF-29610E62CF3D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I3:I10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AF520A82-3C00-40DA-8F14-1EF756F6BE27}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J3:J10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BDB0AC50-6326-4FE2-8EBB-A9645CA60DCF}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3:K10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{56390780-E899-46CA-BB7D-2D0CB4C306C7}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L3:L10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{82AE36BD-71E3-4179-BBA8-F08783EAFE7E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D7B4FE4C-543C-42AB-8CED-20BCB22D01C1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N3:N10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8E53F878-39C8-4364-9202-725B88D49B9D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O3:O10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{59F14498-126E-4615-96AE-185AD5F0025D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{89478E4F-2919-4C59-A4F1-F83163F8AE49}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{86EF0297-B943-4257-AE8A-BC47340A1EEC}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3FF5350B-37FD-4627-AA01-A649A47D3864}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A6E7E027-47DE-4B49-8931-80A2B606B734}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F11:F18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CF525180-9BAE-4A80-9AF8-0A4183AA4731}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G11:G18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{88FC12ED-70BD-4AA3-ABC4-D1638E18C917}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H11:H18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{03C53742-1396-49B5-A75C-B8F2EE6DF507}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I11:I18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E53703C8-6EC4-45AF-A7C5-27EB0E1EDB3C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J11:J18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EC2ACDAC-3433-4298-BB56-4CD282E2FDE1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K11:K18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5F1B9428-DA36-4346-92C6-B774C6ADB83F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L11:L18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8622EB6C-D203-44D6-97DC-BB9E83F74AA9}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M11:M18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{54098384-335C-438C-878E-434B302F1C30}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N11:N18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D7C9DAAE-A316-4507-9935-7E8B7A6D9000}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O11:O18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7305E562-99D7-4701-A3CB-673F89DF4A6E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P11:P18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8721FE99-682B-4CD0-949A-B19E552FB3F2}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P11:P18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7AF7AED4-59B8-40E1-824C-CE7010BF7176}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P11:P18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{38EA70F9-0A79-4BED-8545-D678A2A1186D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P11:P18</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>